<commit_message>
30 pages of documentation, added line_detection_conv section
</commit_message>
<xml_diff>
--- a/Dokumentation/Stand Oster/Vortschritt.xlsx
+++ b/Dokumentation/Stand Oster/Vortschritt.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\Studienarbeit\Dokumentation\Stand Oster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348C721A-62D0-4999-AFD1-79D602E432AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857306B0-5850-4568-84DC-94ED4ECA7CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stand 06_08_2021" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Einleitung</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>VGA Ausgabe</t>
+  </si>
+  <si>
+    <t>Abbildungsverzeichnis</t>
+  </si>
+  <si>
+    <t>Gick Überarbeitung von 04_08</t>
+  </si>
+  <si>
+    <t>Einstellung Threshhold</t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -180,6 +189,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -460,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,148 +501,166 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3"/>
+      <c r="A2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
       <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
+      <c r="A21" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" t="s">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
continued documentation, added OBJECT_DETECTION, DEBUG_OBJECT_DETECTION
</commit_message>
<xml_diff>
--- a/Dokumentation/Stand Oster/Vortschritt.xlsx
+++ b/Dokumentation/Stand Oster/Vortschritt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\Studienarbeit\Dokumentation\Stand Oster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857306B0-5850-4568-84DC-94ED4ECA7CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FE996D-8BFA-45ED-8A5B-83DB66545E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,13 +608,13 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">

</xml_diff>

<commit_message>
added two of three settings in the documentation, added propper title
</commit_message>
<xml_diff>
--- a/Dokumentation/Stand Oster/Vortschritt.xlsx
+++ b/Dokumentation/Stand Oster/Vortschritt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\Studienarbeit\Dokumentation\Stand Oster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FE996D-8BFA-45ED-8A5B-83DB66545E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B343DC8A-E742-4E2F-B5C5-B9B0DD408CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,13 +626,13 @@
       <c r="A21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">

</xml_diff>

<commit_message>
last pushes to finalize documentation before send to review
</commit_message>
<xml_diff>
--- a/Dokumentation/Stand Oster/Vortschritt.xlsx
+++ b/Dokumentation/Stand Oster/Vortschritt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\Studienarbeit\Dokumentation\Stand Oster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B343DC8A-E742-4E2F-B5C5-B9B0DD408CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298ABB67-3F82-4AE8-9656-FE90CC3BDAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stand 06_08_2021" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Einleitung</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Perspektive</t>
-  </si>
-  <si>
-    <t>Einstellung Kamera</t>
   </si>
   <si>
     <t>Funktionsweise/Anknüpfung an Vorheriges</t>
@@ -141,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,8 +163,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -175,11 +178,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -195,6 +213,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -478,7 +497,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,11 +521,11 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -556,7 +575,7 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -579,11 +598,11 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -594,7 +613,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="3"/>
     </row>
@@ -624,7 +643,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -641,10 +660,7 @@
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="9"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>

</xml_diff>